<commit_message>
Added mutex creation to edit mode
</commit_message>
<xml_diff>
--- a/ring.xlsx
+++ b/ring.xlsx
@@ -508,7 +508,11 @@
       <c r="D2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>m312</t>
+        </is>
+      </c>
       <c r="F2" t="n">
         <v>774</v>
       </c>
@@ -552,7 +556,11 @@
       <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E3" t="inlineStr"/>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>m312</t>
+        </is>
+      </c>
       <c r="F3" t="n">
         <v>507</v>
       </c>
@@ -596,7 +604,11 @@
       <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="E4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>m312</t>
+        </is>
+      </c>
       <c r="F4" t="n">
         <v>282</v>
       </c>

</xml_diff>